<commit_message>
Ajustes dos nos artefatos 07, 08, 09, 18, 22 e 23
</commit_message>
<xml_diff>
--- a/Artefatos OPE/22 - Requisitos do Sistema.xlsx
+++ b/Artefatos OPE/22 - Requisitos do Sistema.xlsx
@@ -160,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -179,6 +179,9 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <name val="Arial"/>
     </font>
     <font>
@@ -220,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -234,10 +237,11 @@
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -511,7 +515,7 @@
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -522,7 +526,7 @@
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -533,7 +537,7 @@
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -610,7 +614,7 @@
       <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>